<commit_message>
FAAS-955 Added IRS Specs
</commit_message>
<xml_diff>
--- a/src/test/resources/IRS-8821.xlsx
+++ b/src/test/resources/IRS-8821.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\krish\IdeaProjects\formservice-testing\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{957E5998-BF6B-4A31-8870-493ED9F95405}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57A10C1B-2E13-4639-91DC-08D45CF8AE35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" tabRatio="474" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="31">
   <si>
     <t>useremail</t>
   </si>
@@ -45,14 +45,95 @@
     <t>gsat69101@gmail.com</t>
   </si>
   <si>
-    <t>TEST@GSA1@345</t>
+    <t>VEVTVEBHU0ExQDM0NTY=</t>
+  </si>
+  <si>
+    <t>Taxpayer_firstName</t>
+  </si>
+  <si>
+    <t>Taxpayer_lastName</t>
+  </si>
+  <si>
+    <t>Taxpayer_PhoneNumber</t>
+  </si>
+  <si>
+    <t>Taxpayer_HomeAddress</t>
+  </si>
+  <si>
+    <t>Taxpayer_City</t>
+  </si>
+  <si>
+    <t>Taxpayer_State</t>
+  </si>
+  <si>
+    <t>Taxpayer_Zipcode</t>
+  </si>
+  <si>
+    <t>Taxpayer_IdentityNumber</t>
+  </si>
+  <si>
+    <t>Taxpayer_planNumber</t>
+  </si>
+  <si>
+    <t>Appointee_firstName</t>
+  </si>
+  <si>
+    <t>Appointee_lastName</t>
+  </si>
+  <si>
+    <t>Appointee_phoneNumber</t>
+  </si>
+  <si>
+    <t>Appointee_Address</t>
+  </si>
+  <si>
+    <t>Appointee_City</t>
+  </si>
+  <si>
+    <t>Appointee_State</t>
+  </si>
+  <si>
+    <t>Appointee_Zip</t>
+  </si>
+  <si>
+    <t>Appointee_CFANumber</t>
+  </si>
+  <si>
+    <t>Appointee_PTIN</t>
+  </si>
+  <si>
+    <t>Appointee_FAXNumber</t>
+  </si>
+  <si>
+    <t>Gilmore</t>
+  </si>
+  <si>
+    <t>1667 K Street NW. Washington. DC 20006.</t>
+  </si>
+  <si>
+    <t>Washington</t>
+  </si>
+  <si>
+    <t>DC</t>
+  </si>
+  <si>
+    <t>IRS8821AppointeeFirstName</t>
+  </si>
+  <si>
+    <t>IRS8821AppointeeLastName</t>
+  </si>
+  <si>
+    <t>1800 F Street, NW Washington, DC 20405</t>
+  </si>
+  <si>
+    <t>Miller</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="20" x14ac:knownFonts="1">
+  <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -196,6 +277,14 @@
     <font>
       <sz val="10"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -519,7 +608,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="42">
+  <cellStyleXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
@@ -562,8 +651,9 @@
     <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="16" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -573,13 +663,20 @@
     <xf numFmtId="0" fontId="0" fillId="33" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="19" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="20" fillId="33" borderId="10" xfId="42" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="42">
+  <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
     <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
     <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
@@ -613,6 +710,7 @@
     <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
     <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
     <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Hyperlink" xfId="42" builtinId="8"/>
     <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
     <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
@@ -938,36 +1036,169 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:U2"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B6" sqref="B6"/>
+      <selection pane="bottomRight" activeCell="V18" sqref="V18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
     <col min="1" max="1" width="18.9453125" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.15625" style="6" bestFit="1" customWidth="1"/>
-    <col min="3" max="16384" width="8.83984375" style="1"/>
+    <col min="2" max="2" width="22.62890625" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.20703125" style="8" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.83984375" style="8" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.05078125" style="8" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="34.3671875" style="8" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.20703125" style="8" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.3125" style="8" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.47265625" style="8" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="22.26171875" style="8" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="19.3125" style="8" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="23.47265625" style="8" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="23.26171875" style="8" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="22.15625" style="8" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="33.7890625" style="8" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="13.3671875" style="8" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="14.41796875" style="8" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="12.62890625" style="8" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="20" style="8" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="14" style="8" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="20" style="8" bestFit="1" customWidth="1"/>
+    <col min="22" max="16384" width="8.83984375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:21" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
+      <c r="C1" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="H1" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="J1" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="K1" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="L1" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="M1" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="N1" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="O1" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="P1" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q1" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="R1" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="S1" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="T1" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="U1" s="7" t="s">
+        <v>22</v>
+      </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2" s="7" t="s">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="6" t="s">
         <v>3</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="E2" s="8">
+        <v>2343456321</v>
+      </c>
+      <c r="F2" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="G2" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="H2" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="I2" s="8">
+        <v>20006</v>
+      </c>
+      <c r="J2" s="8">
+        <v>123456789</v>
+      </c>
+      <c r="K2" s="8">
+        <v>1234</v>
+      </c>
+      <c r="L2" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="M2" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="N2" s="8">
+        <v>2223451234</v>
+      </c>
+      <c r="O2" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="P2" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q2" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="R2" s="8">
+        <v>20405</v>
+      </c>
+      <c r="S2" s="8">
+        <v>123456789</v>
+      </c>
+      <c r="T2" s="8">
+        <v>1234</v>
+      </c>
+      <c r="U2" s="8">
+        <v>1111111111</v>
       </c>
     </row>
   </sheetData>
@@ -975,7 +1206,7 @@
   <phoneticPr fontId="18" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1" xr:uid="{3E8BAC91-9B3E-40E9-905A-8071148279DC}"/>
-    <hyperlink ref="B2" r:id="rId2" xr:uid="{6CA1F5F2-F0A3-4E28-9A66-05659123DC63}"/>
+    <hyperlink ref="B2" r:id="rId2" display="TEST@GSA1@3456" xr:uid="{6CA1F5F2-F0A3-4E28-9A66-05659123DC63}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId3"/>

</xml_diff>